<commit_message>
Data can be added to Excel now!
</commit_message>
<xml_diff>
--- a/weather_data.xlsx
+++ b/weather_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Pincode</t>
   </si>
@@ -34,10 +34,22 @@
     <t>Longitude</t>
   </si>
   <si>
+    <t>Temp(c)</t>
+  </si>
+  <si>
+    <t>Temp(f)</t>
+  </si>
+  <si>
     <t>411007</t>
   </si>
   <si>
     <t>Pune City West</t>
+  </si>
+  <si>
+    <t>Udupi</t>
+  </si>
+  <si>
+    <t>Gurgaon</t>
   </si>
 </sst>
 </file>
@@ -395,13 +407,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,13 +432,19 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>6</v>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>411007</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>18.4</v>
@@ -439,6 +457,86 @@
       </c>
       <c r="F2">
         <v>73.87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>576104</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>13.35</v>
+      </c>
+      <c r="F3">
+        <v>74.75</v>
+      </c>
+      <c r="G3">
+        <v>25</v>
+      </c>
+      <c r="H3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>122101</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>28.47</v>
+      </c>
+      <c r="F4">
+        <v>77.03</v>
+      </c>
+      <c r="G4">
+        <v>14</v>
+      </c>
+      <c r="H4">
+        <v>57.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>122003</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>28.47</v>
+      </c>
+      <c r="F5">
+        <v>77.03</v>
+      </c>
+      <c r="G5">
+        <v>14</v>
+      </c>
+      <c r="H5">
+        <v>57.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>18.53</v>
+      </c>
+      <c r="F6">
+        <v>73.87</v>
+      </c>
+      <c r="G6">
+        <v>17.4</v>
+      </c>
+      <c r="H6">
+        <v>63.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>